<commit_message>
feat: Complete Phase 6 with E2E test infrastructure
## Phase 6 - Advanced Features
- Knowledge Graph testset generation (kg_generator, entity_extractor)
- Experiment management system (experiment.py, experiment_manager.py)
- Multilingual prompts (Japanese, Chinese support)
- PostgreSQL storage adapter
- MLflow tracker adapter
- Azure OpenAI adapter
- Anthropic Claude adapter

## E2E Test Infrastructure
- Multi-format test fixtures (JSON, CSV, XLSX)
- Comprehensive E2E test scenarios (27 tests)
- pytest-html report generation
- Persistent evaluation result storage (data/e2e_results/)
- JUnit XML output for CI/CD integration

## Test Coverage
- Unit tests: 354
- Integration tests: 53
- Total: 407 tests passing

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tests/fixtures/sample_dataset.xlsx
+++ b/tests/fixtures/sample_dataset.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test_cases" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,27 +422,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>question</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>answer</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>contexts</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>ground_truth</t>
         </is>
@@ -559,7 +547,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Test-Driven Development|Write tests first|Red-Green-Refactor cycle</t>
+          <t>["Test-Driven Development", "Write tests first", "Red-Green-Refactor cycle"]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">

</xml_diff>